<commit_message>
cmabio la linea 9
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nahuel Valverde\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A27B15A-83EE-49DE-9B77-F7CA64033B61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Tareas" sheetId="1" r:id="rId1"/>
@@ -72,9 +66,6 @@
   </si>
   <si>
     <t>Se abona el plan de prueba 03 y se constata después de correr los scripts que el usuario queda en esta CORRECTO</t>
-  </si>
-  <si>
-    <t>Pasaje estado CORRECTO a DEUDA: ingresar pero no pagar periodo actual (esperar vencimiento)</t>
   </si>
   <si>
     <t xml:space="preserve">Pasaje estado DEUDA a DEUDA: esperar vencimiento para verificar que continua la deuda
@@ -222,11 +213,14 @@
   <si>
     <t>Franco Gabriel Comisso</t>
   </si>
+  <si>
+    <t>Pasaje estado En proceso</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d&quot;-&quot;mmm&quot;-&quot;"/>
   </numFmts>
@@ -845,19 +839,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AA999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="77.140625" customWidth="1"/>
+    <col min="1" max="1" width="79" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="74.28515625" customWidth="1"/>
   </cols>
@@ -991,7 +985,7 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="B9" s="15">
         <v>7</v>
@@ -1001,7 +995,7 @@
     </row>
     <row r="10" spans="1:27" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="18">
         <v>8</v>
@@ -1011,7 +1005,7 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="21">
         <v>9</v>
@@ -1021,7 +1015,7 @@
     </row>
     <row r="12" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="23">
         <v>10</v>
@@ -1031,7 +1025,7 @@
     </row>
     <row r="13" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="21">
         <v>11</v>
@@ -1041,7 +1035,7 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="23">
         <v>12</v>
@@ -1051,7 +1045,7 @@
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="21">
         <v>13</v>
@@ -1061,7 +1055,7 @@
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="23">
         <v>14</v>
@@ -1071,7 +1065,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="21">
         <v>15</v>
@@ -5186,7 +5180,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -5209,7 +5203,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
@@ -5220,36 +5214,36 @@
     </row>
     <row r="2" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="C2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="D2" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="E2" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="F2" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="G2" s="36" t="s">
         <v>31</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="C3" s="38" t="s">
         <v>34</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>35</v>
       </c>
       <c r="D3" s="39">
         <v>43818</v>
@@ -5260,13 +5254,13 @@
     </row>
     <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="44" t="s">
         <v>34</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>35</v>
       </c>
       <c r="D4" s="45">
         <v>43818</v>
@@ -5277,13 +5271,13 @@
     </row>
     <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="39">
         <v>43818</v>
@@ -5294,13 +5288,13 @@
     </row>
     <row r="6" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="43" t="s">
-        <v>39</v>
-      </c>
       <c r="C6" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="45">
         <v>43818</v>
@@ -5311,13 +5305,13 @@
     </row>
     <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="39">
         <v>43818</v>
@@ -5328,13 +5322,13 @@
     </row>
     <row r="8" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="45">
         <v>43818</v>
@@ -5345,13 +5339,13 @@
     </row>
     <row r="9" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="39">
         <v>43818</v>
@@ -5362,13 +5356,13 @@
     </row>
     <row r="10" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="45">
         <v>43818</v>
@@ -5379,13 +5373,13 @@
     </row>
     <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="39">
         <v>43818</v>
@@ -5396,13 +5390,13 @@
     </row>
     <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="45">
         <v>43818</v>
@@ -5413,13 +5407,13 @@
     </row>
     <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="39">
         <v>43818</v>
@@ -5430,13 +5424,13 @@
     </row>
     <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="43" t="s">
         <v>34</v>
-      </c>
-      <c r="C14" s="43" t="s">
-        <v>35</v>
       </c>
       <c r="D14" s="45">
         <v>43818</v>
@@ -5447,13 +5441,13 @@
     </row>
     <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="39">
         <v>43818</v>
@@ -5464,13 +5458,13 @@
     </row>
     <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="45">
         <v>43818</v>
@@ -5481,13 +5475,13 @@
     </row>
     <row r="17" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="39">
         <v>43818</v>
@@ -5498,13 +5492,13 @@
     </row>
     <row r="18" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="45">
         <v>43818</v>
@@ -5515,13 +5509,13 @@
     </row>
     <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="38" t="s">
         <v>34</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>35</v>
       </c>
       <c r="D19" s="39">
         <v>43818</v>
@@ -5532,13 +5526,13 @@
     </row>
     <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="45">
         <v>43818</v>
@@ -5549,13 +5543,13 @@
     </row>
     <row r="21" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="39">
         <v>43818</v>
@@ -5566,13 +5560,13 @@
     </row>
     <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="45">
         <v>43818</v>
@@ -5583,13 +5577,13 @@
     </row>
     <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="39">
         <v>43818</v>
@@ -5600,13 +5594,13 @@
     </row>
     <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="43" t="s">
         <v>34</v>
-      </c>
-      <c r="C24" s="43" t="s">
-        <v>35</v>
       </c>
       <c r="D24" s="45">
         <v>43818</v>
@@ -5617,13 +5611,13 @@
     </row>
     <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="38" t="s">
         <v>34</v>
-      </c>
-      <c r="C25" s="38" t="s">
-        <v>35</v>
       </c>
       <c r="D25" s="39">
         <v>43818</v>
@@ -5634,13 +5628,13 @@
     </row>
     <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="45">
         <v>43818</v>
@@ -5651,13 +5645,13 @@
     </row>
     <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D27" s="39">
         <v>43818</v>
@@ -5668,13 +5662,13 @@
     </row>
     <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="45">
         <v>43818</v>
@@ -5685,13 +5679,13 @@
     </row>
     <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" s="39">
         <v>43818</v>
@@ -5702,13 +5696,13 @@
     </row>
     <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="20" t="s">
         <v>34</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>35</v>
       </c>
       <c r="D30" s="45">
         <v>43818</v>
@@ -5719,13 +5713,13 @@
     </row>
     <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" s="50">
         <v>43826</v>
@@ -10256,7 +10250,7 @@
       <c r="E1000" s="32"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G31" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A2:G31"/>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>

</xml_diff>